<commit_message>
Updated the Excel TC002
</commit_message>
<xml_diff>
--- a/data/TC002.xlsx
+++ b/data/TC002.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vidhyananth\eclipse-workspace\ACMESystemPOMFramework\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E644AC94-5742-40B2-8890-FE4233BA5A7F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88338DD6-1A67-4751-9881-220EBFB4A0C6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>UserName</t>
   </si>
@@ -33,22 +33,10 @@
     <t>Password</t>
   </si>
   <si>
-    <t>VendorName</t>
-  </si>
-  <si>
     <t>kumar.testleaf@gmail.com</t>
   </si>
   <si>
     <t>leaf@12</t>
-  </si>
-  <si>
-    <t>Blue Lagoon</t>
-  </si>
-  <si>
-    <t>CountryName</t>
-  </si>
-  <si>
-    <t>France</t>
   </si>
 </sst>
 </file>
@@ -377,45 +365,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="S5" sqref="S5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="23.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>